<commit_message>
more recent unfolding experiment
</commit_message>
<xml_diff>
--- a/Data/2016/03_March/20160329_WWRQ_45_Bradford_TN_REPLICATE_quant.xlsx
+++ b/Data/2016/03_March/20160329_WWRQ_45_Bradford_TN_REPLICATE_quant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="-25760" yWindow="4120" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,8 +136,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -130,7 +150,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,11 +521,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2119430136"/>
-        <c:axId val="-2101229160"/>
+        <c:axId val="-2101294760"/>
+        <c:axId val="-2085659624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2119430136"/>
+        <c:axId val="-2101294760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,12 +554,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2101229160"/>
+        <c:crossAx val="-2085659624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2101229160"/>
+        <c:axId val="-2085659624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119430136"/>
+        <c:crossAx val="-2101294760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -824,11 +848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2084429288"/>
-        <c:axId val="-2087263800"/>
+        <c:axId val="-2097370424"/>
+        <c:axId val="-2097218136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2084429288"/>
+        <c:axId val="-2097370424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,12 +886,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087263800"/>
+        <c:crossAx val="-2097218136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2087263800"/>
+        <c:axId val="-2097218136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,7 +925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084429288"/>
+        <c:crossAx val="-2097370424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1149,11 +1173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2118209720"/>
-        <c:axId val="-2121677016"/>
+        <c:axId val="-2100528168"/>
+        <c:axId val="-2085804056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2118209720"/>
+        <c:axId val="-2100528168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,12 +1211,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121677016"/>
+        <c:crossAx val="-2085804056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2121677016"/>
+        <c:axId val="-2085804056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118209720"/>
+        <c:crossAx val="-2100528168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1474,11 +1498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2084680488"/>
-        <c:axId val="-2085138904"/>
+        <c:axId val="2080527960"/>
+        <c:axId val="2080537576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2084680488"/>
+        <c:axId val="2080527960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,12 +1536,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085138904"/>
+        <c:crossAx val="2080537576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2085138904"/>
+        <c:axId val="2080537576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084680488"/>
+        <c:crossAx val="2080527960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1895,11 +1919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2120089544"/>
-        <c:axId val="-2119231576"/>
+        <c:axId val="-2121932088"/>
+        <c:axId val="-2122087656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2120089544"/>
+        <c:axId val="-2121932088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,13 +1957,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119231576"/>
+        <c:crossAx val="-2122087656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2119231576"/>
+        <c:axId val="-2122087656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120089544"/>
+        <c:crossAx val="-2121932088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2475,7 +2499,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="L16" sqref="L16:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3185,7 +3209,7 @@
         <v>0.43916349809885941</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" ref="Q21:R21" si="14">(((M8+0.0227)/0.0501)/10)</f>
+        <f t="shared" ref="Q21" si="14">(((M8+0.0227)/0.0501)/10)</f>
         <v>0.95948103792415174</v>
       </c>
       <c r="R21" s="1"/>
@@ -3377,6 +3401,7 @@
     <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>